<commit_message>
Data model for Seven Sages Brewing Company in progress update
</commit_message>
<xml_diff>
--- a/Udacity Preparing and Modelling Data/Data Model for Seven Sages Brewing Company/source-files/Monthly Sales Logs/SSBC - Apr 2021 Sales.xlsx
+++ b/Udacity Preparing and Modelling Data/Data Model for Seven Sages Brewing Company/source-files/Monthly Sales Logs/SSBC - Apr 2021 Sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PowerBI\Power-BI\Udacity Preparing and Modelling Data\Data Model for Seven Sages Brewing Company\source-files\Monthly Sales Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E0278C-DE5A-46C6-9D1D-CB2CF43408E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F03D84-C276-4448-B0D3-F001960F0128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2544" windowWidth="23256" windowHeight="13176" xr2:uid="{AE05B252-52D3-4C12-A85B-E21020B19BF7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{AE05B252-52D3-4C12-A85B-E21020B19BF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Apr 2021 Sales" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>SSBC3004</t>
-  </si>
-  <si>
-    <t>CAD</t>
   </si>
   <si>
     <t>SSBC3002</t>
@@ -394,7 +391,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AB61711-DCA2-4C8B-BC48-13133F72FD24}" name="Table53711" displayName="Table53711" ref="A1:E64" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E64" xr:uid="{5FADBE7F-BA1B-4A37-90C5-0AFE3140F2F2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BD189298-0682-49BA-AA0F-6630D2DEDB5F}" name="CustID" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{E915BF2B-EFAF-4BE5-A38A-2442F0A2691E}" name="ProdID" dataDxfId="3"/>
@@ -708,20 +704,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -733,7 +729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -744,14 +740,14 @@
         <v>44288</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f t="shared" ref="D2:D51" si="0">IF(LEFT(A2,2)="BC","CAD","USD")</f>
+        <f t="shared" ref="D2:D64" si="0">IF(LEFT(A2,2)="BC","CAD","USD")</f>
         <v>CAD</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -769,7 +765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -787,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -805,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -823,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -841,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -859,7 +855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -877,7 +873,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -895,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -913,7 +909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -931,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -949,7 +945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -967,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -985,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1021,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1039,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +1053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1075,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1093,7 +1089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1111,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1129,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1147,7 +1143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1165,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1183,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -1201,7 +1197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1219,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1237,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -1255,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1291,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1309,7 +1305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -1327,7 +1323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -1345,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1363,7 +1359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -1381,7 +1377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
@@ -1417,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
@@ -1453,7 +1449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -1471,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
@@ -1489,7 +1485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -1507,7 +1503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -1543,7 +1539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -1561,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -1579,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -1597,7 +1593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -1615,7 +1611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -1633,7 +1629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>15</v>
       </c>
@@ -1644,14 +1640,14 @@
         <v>44296</v>
       </c>
       <c r="D52" s="1" t="str">
-        <f>IF(LEFT(A52,2)="BC","CAD","USD")</f>
+        <f t="shared" si="0"/>
         <v>USD</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>27</v>
       </c>
@@ -1662,14 +1658,14 @@
         <v>44296</v>
       </c>
       <c r="D53" s="1" t="str">
-        <f t="shared" ref="D53:D54" si="1">IF(LEFT(A53,2)="BC","CAD","USD")</f>
+        <f t="shared" si="0"/>
         <v>USD</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>19</v>
       </c>
@@ -1680,14 +1676,14 @@
         <v>44296</v>
       </c>
       <c r="D54" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>USD</v>
       </c>
       <c r="E54" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>15</v>
       </c>
@@ -1698,14 +1694,14 @@
         <v>44311</v>
       </c>
       <c r="D55" s="1" t="str">
-        <f>IF(LEFT(A55,2)="BC","CAD","USD")</f>
+        <f t="shared" si="0"/>
         <v>USD</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>27</v>
       </c>
@@ -1716,14 +1712,14 @@
         <v>44311</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f t="shared" ref="D56:D59" si="2">IF(LEFT(A56,2)="BC","CAD","USD")</f>
+        <f t="shared" si="0"/>
         <v>USD</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>19</v>
       </c>
@@ -1734,14 +1730,14 @@
         <v>44311</v>
       </c>
       <c r="D57" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>USD</v>
       </c>
       <c r="E57" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>17</v>
       </c>
@@ -1751,15 +1747,15 @@
       <c r="C58" s="2">
         <v>44300</v>
       </c>
-      <c r="D58" s="5" t="str">
-        <f t="shared" si="2"/>
+      <c r="D58" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>CAD</v>
       </c>
       <c r="E58" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>19</v>
       </c>
@@ -1769,15 +1765,15 @@
       <c r="C59" s="2">
         <v>44301</v>
       </c>
-      <c r="D59" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="D59" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>USD</v>
       </c>
       <c r="E59" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
@@ -1787,31 +1783,33 @@
       <c r="C60" s="2">
         <v>44302</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>30</v>
+      <c r="D60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CAD</v>
       </c>
       <c r="E60" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C61" s="2">
         <v>44303</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>30</v>
+      <c r="D61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CAD</v>
       </c>
       <c r="E61" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -1821,49 +1819,49 @@
       <c r="C62" s="2">
         <v>44304</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>30</v>
+      <c r="D62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CAD</v>
       </c>
       <c r="E62" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C63" s="2">
         <v>44305</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>30</v>
+      <c r="D63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CAD</v>
       </c>
       <c r="E63" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C64" s="2">
         <v>44306</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>30</v>
+      <c r="D64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CAD</v>
       </c>
       <c r="E64" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>